<commit_message>
updated the fig1 script and removed extra files
</commit_message>
<xml_diff>
--- a/result/cell_line_per_tissue.xlsx
+++ b/result/cell_line_per_tissue.xlsx
@@ -381,7 +381,7 @@
         </is>
       </c>
       <c r="B2">
-        <v>24</v>
+        <v>98</v>
       </c>
       <c r="C2">
         <v>78</v>
@@ -394,7 +394,7 @@
         </is>
       </c>
       <c r="B3">
-        <v>17</v>
+        <v>30</v>
       </c>
       <c r="C3">
         <v>49</v>
@@ -407,7 +407,7 @@
         </is>
       </c>
       <c r="B4">
-        <v>59</v>
+        <v>128</v>
       </c>
       <c r="C4">
         <v>94</v>
@@ -420,7 +420,7 @@
         </is>
       </c>
       <c r="B5">
-        <v>40</v>
+        <v>59</v>
       </c>
       <c r="C5">
         <v>53</v>
@@ -433,7 +433,7 @@
         </is>
       </c>
       <c r="B6">
-        <v>144</v>
+        <v>72</v>
       </c>
       <c r="C6">
         <v>71</v>
@@ -446,7 +446,7 @@
         </is>
       </c>
       <c r="B7">
-        <v>71</v>
+        <v>101</v>
       </c>
       <c r="C7">
         <v>107</v>
@@ -459,7 +459,7 @@
         </is>
       </c>
       <c r="B8">
-        <v>20</v>
+        <v>41</v>
       </c>
       <c r="C8">
         <v>33</v>
@@ -472,7 +472,7 @@
         </is>
       </c>
       <c r="B9">
-        <v>22</v>
+        <v>26</v>
       </c>
       <c r="C9">
         <v>19</v>
@@ -485,7 +485,7 @@
         </is>
       </c>
       <c r="B10">
-        <v>147</v>
+        <v>198</v>
       </c>
       <c r="C10">
         <v>193</v>
@@ -498,7 +498,7 @@
         </is>
       </c>
       <c r="B11">
-        <v>219</v>
+        <v>240</v>
       </c>
       <c r="C11">
         <v>243</v>
@@ -511,7 +511,7 @@
         </is>
       </c>
       <c r="B12">
-        <v>38</v>
+        <v>47</v>
       </c>
       <c r="C12">
         <v>33</v>
@@ -524,7 +524,7 @@
         </is>
       </c>
       <c r="B13">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="C13">
         <v>13</v>
@@ -537,7 +537,7 @@
         </is>
       </c>
       <c r="B14">
-        <v>51</v>
+        <v>62</v>
       </c>
       <c r="C14">
         <v>63</v>
@@ -550,7 +550,7 @@
         </is>
       </c>
       <c r="B15">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="C15">
         <v>18</v>
@@ -563,7 +563,7 @@
         </is>
       </c>
       <c r="B16">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C16">
         <v>17</v>

</xml_diff>